<commit_message>
Funcion para importar egresados
</commit_message>
<xml_diff>
--- a/bak_formato_alumnos_excel.xlsx
+++ b/bak_formato_alumnos_excel.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Egresados" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>carnet</t>
   </si>
@@ -56,16 +56,19 @@
     <t>direccion</t>
   </si>
   <si>
+    <t>carreras</t>
+  </si>
+  <si>
     <t>2009-30761</t>
   </si>
   <si>
     <t>161-090392-0001Q</t>
   </si>
   <si>
-    <t>miguel angel</t>
-  </si>
-  <si>
-    <t>castillo cornejo</t>
+    <t>Miguel Angel</t>
+  </si>
+  <si>
+    <t>Castillo Cornejo</t>
   </si>
   <si>
     <t>M</t>
@@ -74,37 +77,25 @@
     <t>mikedosce1992@gmail.com</t>
   </si>
   <si>
-    <t>ant mol 2000 75 vrs al Oeste</t>
-  </si>
-  <si>
-    <t>2099-30789</t>
-  </si>
-  <si>
-    <t>001-030292-0062E</t>
-  </si>
-  <si>
-    <t>rene mauricio</t>
-  </si>
-  <si>
-    <t>cruz hernandez</t>
-  </si>
-  <si>
-    <t>reneblackr@gmail.com</t>
-  </si>
-  <si>
-    <t>del tamarindo 2 c al guindo</t>
-  </si>
-  <si>
-    <t>Ingenieria industrial</t>
+    <t>antiguos molinos 2000 75 vrs al Oeste</t>
   </si>
   <si>
     <t>Ingeniería de sistemas</t>
   </si>
   <si>
-    <t>Ingeniería otra asdsa1</t>
-  </si>
-  <si>
-    <t>carreras</t>
+    <t>2008-89012</t>
+  </si>
+  <si>
+    <t>Jose Alberto</t>
+  </si>
+  <si>
+    <t>Molina</t>
+  </si>
+  <si>
+    <t>jose_molina@gmail.com</t>
+  </si>
+  <si>
+    <t>Ingeniería de agropecuaria</t>
   </si>
 </sst>
 </file>
@@ -173,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -186,9 +177,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -197,6 +185,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -479,21 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
     <col min="11" max="11" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -529,124 +524,113 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6">
+        <v>15</v>
+      </c>
+      <c r="F2" s="9">
         <v>33672</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="5">
         <v>27322264</v>
       </c>
       <c r="I2" s="5">
-        <v>84944968</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>23</v>
+        <v>89021739</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6">
-        <v>33637</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="5">
-        <v>27136727</v>
-      </c>
-      <c r="I3" s="5">
-        <v>89469271</v>
-      </c>
-      <c r="J3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9">
+        <v>38876</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>24</v>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="6">
-        <v>33637</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="5">
-        <v>27136727</v>
-      </c>
-      <c r="I4" s="5">
-        <v>89469271</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="6"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="6"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J14" s="2"/>
     </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Gif de carga en enviar mensajes
</commit_message>
<xml_diff>
--- a/bak_formato_alumnos_excel.xlsx
+++ b/bak_formato_alumnos_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>carnet</t>
   </si>
@@ -96,6 +96,30 @@
   </si>
   <si>
     <t>Ingeniería de agropecuaria</t>
+  </si>
+  <si>
+    <t>Cristina Maria</t>
+  </si>
+  <si>
+    <t>Leiva Fajardo</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>leivafajardo@gmail.com</t>
+  </si>
+  <si>
+    <t>La concha de la lora</t>
+  </si>
+  <si>
+    <t>171-090392-0001Q</t>
+  </si>
+  <si>
+    <t>161-090392-0001F</t>
+  </si>
+  <si>
+    <t>2009-30746</t>
   </si>
 </sst>
 </file>
@@ -477,7 +501,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +590,9 @@
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
@@ -590,17 +616,35 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="9">
+        <v>33765</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -629,8 +673,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configuracion de privacidad insertada al importar egresados
</commit_message>
<xml_diff>
--- a/bak_formato_alumnos_excel.xlsx
+++ b/bak_formato_alumnos_excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>carnet</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>2009-30746</t>
+  </si>
+  <si>
+    <t>2009-89034</t>
+  </si>
+  <si>
+    <t>Randall</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>randall@gmail.com</t>
+  </si>
+  <si>
+    <t>adasddasdsa</t>
   </si>
 </sst>
 </file>
@@ -501,7 +516,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,13 +662,28 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="6"/>
-      <c r="K5" s="5"/>
+      <c r="G5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
@@ -674,8 +704,9 @@
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1"/>
     <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>